<commit_message>
changed theme to dark black1. added brands list to combo box from base.xlsx.
added base parameters in models. trying to make depended list in model dropbox

Interface fully working with popup generated code with 4th number that sign count of manager in list. For now after press ok prog making writing in file. controlling unfilled fields

created exe file
</commit_message>
<xml_diff>
--- a/base/base.xlsx
+++ b/base/base.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ЭтаКнига"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7850" tabRatio="600" firstSheet="1" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_conditions" sheetId="1" state="visible" r:id="rId1"/>
@@ -448,9 +448,9 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="14.42578125" customWidth="1" min="2" max="8"/>
+    <col width="14.453125" customWidth="1" min="2" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -690,7 +690,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -754,9 +754,9 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="11.140625" customWidth="1" min="1" max="1"/>
+    <col width="11.1796875" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1053,10 +1053,10 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1085,7 +1085,7 @@
         <v>200000</v>
       </c>
       <c r="C2" t="n">
-        <v>197000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="3">
@@ -1124,7 +1124,7 @@
         <v>150000</v>
       </c>
       <c r="C5" t="n">
-        <v>150000</v>
+        <v>148200</v>
       </c>
     </row>
     <row r="6">
@@ -1171,9 +1171,9 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="13.42578125" customWidth="1" min="2" max="2"/>
+    <col width="13.453125" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1272,7 +1272,7 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1659,7 +1659,7 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1762,7 +1762,7 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>